<commit_message>
service 09 itid 01-08
</commit_message>
<xml_diff>
--- a/dbc.xlsx
+++ b/dbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27135" windowHeight="12525" activeTab="2"/>
+    <workbookView windowWidth="27135" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="dbcmap" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6666" uniqueCount="2768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6667" uniqueCount="2768">
   <si>
     <t>Little Endian</t>
   </si>
@@ -10165,8 +10165,8 @@
   <sheetPr/>
   <dimension ref="A2:BN6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG3" sqref="Z2:AG3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="5"/>
@@ -10528,7 +10528,9 @@
       <c r="BC5" s="92"/>
       <c r="BD5" s="92"/>
       <c r="BE5" s="92"/>
-      <c r="BF5" s="92"/>
+      <c r="BF5" s="92" t="s">
+        <v>1</v>
+      </c>
       <c r="BG5" s="92"/>
       <c r="BH5" s="92"/>
       <c r="BI5" s="92"/>
@@ -12286,10 +12288,10 @@
   <sheetPr/>
   <dimension ref="A1:P1304"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="E1201" sqref="E1201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>

</xml_diff>